<commit_message>
60V_IND and BSPD RTM
</commit_message>
<xml_diff>
--- a/60V_IND/Altium/Project Outputs for 60V_Ind/BOM/Bill of Materials-60V_Ind.xlsx
+++ b/60V_IND/Altium/Project Outputs for 60V_Ind/BOM/Bill of Materials-60V_Ind.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\AERO_2019-2020\60V_IND\Project Outputs for 60V_Ind\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\AERO_2019-2020\60V_IND\Altium\Project Outputs for 60V_Ind\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89EF89FB-C95E-42E0-A5D9-0B9B8FC53426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DF012F6-EB31-427A-988E-AA657E105BC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="34560" windowHeight="18684" xr2:uid="{174C0748-6BA0-4EAE-BBB3-8A0C8A0FD70B}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15435" xr2:uid="{B5E08E63-A122-4805-86BA-5F1B6C2E006B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-60V_Ind" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
   <si>
     <t>Line #</t>
   </si>
@@ -92,10 +92,7 @@
     <t>C1</t>
   </si>
   <si>
-    <t>CMP-2000-05454-1</t>
-  </si>
-  <si>
-    <t>Released</t>
+    <t>Unknown server</t>
   </si>
   <si>
     <t>TDK</t>
@@ -630,7 +627,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C0642E-2DAC-4779-8A80-FE556896F8EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46B5609-DD4D-40E4-8145-E8AAB14CE8B0}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -638,24 +635,24 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="45" customWidth="1"/>
-    <col min="4" max="5" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="26.44140625" customWidth="1"/>
-    <col min="10" max="10" width="23.109375" customWidth="1"/>
-    <col min="11" max="11" width="12.21875" customWidth="1"/>
-    <col min="12" max="12" width="22.33203125" customWidth="1"/>
-    <col min="13" max="13" width="20.109375" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" customWidth="1"/>
+    <col min="4" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" customWidth="1"/>
+    <col min="10" max="10" width="24" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -699,7 +696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -712,29 +709,27 @@
       <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="G2" s="4">
         <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="M2" s="4">
         <v>0.55000000000000004</v>
@@ -743,40 +738,40 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="4">
         <v>1</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="M3" s="4">
         <v>0.56999999999999995</v>
@@ -785,40 +780,40 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" s="4">
         <v>2</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="M4" s="4">
         <v>1.22</v>
@@ -827,40 +822,40 @@
         <v>2.44</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="4">
         <v>1</v>
       </c>
       <c r="H5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="M5" s="4">
         <v>1.61</v>
@@ -869,40 +864,40 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="4">
         <v>1</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="L6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M6" s="4">
         <v>0.69</v>
@@ -911,40 +906,40 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="4">
         <v>1</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="L7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M7" s="4">
         <v>0.56999999999999995</v>
@@ -953,40 +948,40 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="4">
         <v>4</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="L8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M8" s="4">
         <v>0.11</v>
@@ -995,40 +990,40 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="4">
         <v>1</v>
       </c>
       <c r="H9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="M9" s="4">
         <v>0.1</v>
@@ -1037,40 +1032,40 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="4">
         <v>1</v>
       </c>
       <c r="H10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="M10" s="4">
         <v>0.93</v>
@@ -1082,6 +1077,6 @@
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="51" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="49" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>